<commit_message>
completed the python main libraries
</commit_message>
<xml_diff>
--- a/code_script_notebooks/jupyter_notebooks/sample.xlsx
+++ b/code_script_notebooks/jupyter_notebooks/sample.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,12 +426,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>42</v>
+        <v>52879</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>44987.66474087031</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
@@ -440,6 +440,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>44987.76033516775</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>